<commit_message>
More functionality added to MagentoSTB Project
</commit_message>
<xml_diff>
--- a/MagentoSTB/testData/inputExcel.xlsx
+++ b/MagentoSTB/testData/inputExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Project\MagentoSTB\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC88D2-2612-4BA1-B273-B6B9D90AFF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3252C1-E15E-4FE4-8DA4-88B0064127DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A55EEF25-6765-4F26-A9F2-9C420C671F4A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -52,16 +52,91 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>End to End Test 1</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Men Jacket,Men Pants,Men Tanks,Women Tees</t>
+  </si>
+  <si>
+    <t>Beaumont Summit Kit,Geo Insulated Jogging Pant,Rocco Gym Tank,Layla Tee</t>
+  </si>
+  <si>
+    <t>Sizes</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>L,34,M,S</t>
+  </si>
+  <si>
+    <t>Red,Green,Blue,Red</t>
+  </si>
+  <si>
+    <t>2,1,2,1</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Add to Cart</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Add and Remove from Cart</t>
+  </si>
+  <si>
+    <t>Women Bras&amp;Tanks</t>
+  </si>
+  <si>
+    <t>Celeste Sports Bra</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Products to Add</t>
+  </si>
+  <si>
+    <t>QuantityToAdd</t>
+  </si>
+  <si>
+    <t>QuantityToRemove</t>
+  </si>
+  <si>
+    <t>Products to Remove</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -415,20 +490,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F0C730-F84C-435F-91ED-7DCF2AE2EDC1}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +519,29 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -447,10 +549,95 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More POM Pages added to MagentoSTB Project
</commit_message>
<xml_diff>
--- a/MagentoSTB/testData/inputExcel.xlsx
+++ b/MagentoSTB/testData/inputExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Project\MagentoSTB\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3252C1-E15E-4FE4-8DA4-88B0064127DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADDF853-5C91-482F-8BF9-CB026CF3AF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A55EEF25-6765-4F26-A9F2-9C420C671F4A}"/>
+    <workbookView xWindow="4236" yWindow="2472" windowWidth="17280" windowHeight="8880" xr2:uid="{A55EEF25-6765-4F26-A9F2-9C420C671F4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>Add and Remove from Cart</t>
   </si>
   <si>
-    <t>Women Bras&amp;Tanks</t>
-  </si>
-  <si>
     <t>Celeste Sports Bra</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Products to Remove</t>
+  </si>
+  <si>
+    <t>Women Bras &amp; Tanks</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +523,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -532,13 +532,13 @@
         <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -563,16 +563,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="2">
         <v>2</v>
@@ -589,22 +589,22 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>

</xml_diff>